<commit_message>
Added data from Nov 8
</commit_message>
<xml_diff>
--- a/MFC_Tests/MFC_Data_Cheatsheet/MFC_Data_Cheatsheet.xlsx
+++ b/MFC_Tests/MFC_Data_Cheatsheet/MFC_Data_Cheatsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="124">
   <si>
     <t>EntryNumber</t>
   </si>
@@ -358,6 +358,30 @@
   </si>
   <si>
     <t>10/26/2022 - Board2 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>11/03/2022 - Board0 - NO, RH</t>
+  </si>
+  <si>
+    <t>11/03/2022 - Board1 - NO, RH</t>
+  </si>
+  <si>
+    <t>11/04/2022 - Board0 - NO, RH</t>
+  </si>
+  <si>
+    <t>11/07/2022 - Board0 - N2O, RH</t>
+  </si>
+  <si>
+    <t>11/07/2022 - Board0 - N2O, RH Permselect</t>
+  </si>
+  <si>
+    <t>11/07/2022 - Board0 - N2O, RH Permselect, PostSCUID</t>
+  </si>
+  <si>
+    <t>11/08/2022 - Board0 - N2O, RH Permselect, Air</t>
+  </si>
+  <si>
+    <t>11/08/2022 - Board0 - N2O, RH Permselect</t>
   </si>
   <si>
     <t>ExtraComments</t>
@@ -406,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E108"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="true"/>
@@ -430,7 +454,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2">
@@ -1918,6 +1942,126 @@
       </c>
       <c r="E100" s="0"/>
     </row>
+    <row r="101">
+      <c r="A101" s="0">
+        <v>101</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="0">
+        <v>21</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E101" s="0"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="0">
+        <v>102</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="0">
+        <v>22</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E102" s="0"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="0">
+        <v>103</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="0">
+        <v>21</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E103" s="0"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="0">
+        <v>104</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104" s="0">
+        <v>21</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E104" s="0"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="0">
+        <v>105</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="0">
+        <v>21</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E105" s="0"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="0">
+        <v>106</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106" s="0">
+        <v>21</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E106" s="0"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="0">
+        <v>107</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="0">
+        <v>22</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E107" s="0"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="0">
+        <v>108</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="0">
+        <v>22</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E108" s="0"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>